<commit_message>
35 Head of account moved from table to header
</commit_message>
<xml_diff>
--- a/MAS.Web/wwwroot/report/ujjain store/MAS Account.xlsx
+++ b/MAS.Web/wwwroot/report/ujjain store/MAS Account.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ujjain store</t>
   </si>
@@ -110,6 +110,30 @@
     <t>Received during the month</t>
   </si>
   <si>
+    <t>15.08.2017</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Pitamber Jain, MB M-902, Page 12, Ag 902, W.O w-902</t>
+  </si>
+  <si>
+    <t>Punji Lal</t>
+  </si>
+  <si>
+    <t>31.08.2017</t>
+  </si>
+  <si>
+    <t>43214 / 04.08.2017</t>
+  </si>
+  <si>
+    <t>Mohan lal makhan</t>
+  </si>
+  <si>
+    <t>hod acc</t>
+  </si>
+  <si>
     <t>Total Received during the month</t>
   </si>
   <si>
@@ -117,6 +141,18 @@
   </si>
   <si>
     <t>Issue during the month</t>
+  </si>
+  <si>
+    <t>14.08.2017</t>
+  </si>
+  <si>
+    <t>602 / 10.08.2017</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>Punji Head</t>
   </si>
   <si>
     <t>Total Issue during the month</t>
@@ -130,7 +166,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -148,6 +184,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -225,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="1" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -267,6 +307,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" applyNumberFormat="1" fontId="2" applyFont="1" borderId="7" applyBorder="1" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" borderId="7" applyBorder="1" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="4" applyFont="1" borderId="7" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="7" applyBorder="1" xfId="0"/>
@@ -280,7 +326,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -534,16 +580,16 @@
         <v>30</v>
       </c>
       <c r="E7" s="14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F7" s="14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G7" s="14">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H7" s="14">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I7" s="14">
         <v>0</v>
@@ -571,187 +617,265 @@
       <c r="D8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="14">
-        <f>SUM(E9:E8)</f>
-      </c>
-      <c r="F9" s="14">
-        <f>SUM(F9:F8)</f>
-      </c>
-      <c r="G9" s="14">
-        <f>SUM(G9:G8)</f>
-      </c>
-      <c r="H9" s="14">
-        <f>SUM(H9:H8)</f>
-      </c>
-      <c r="I9" s="14">
-        <f>SUM(I9:I8)</f>
-      </c>
-      <c r="J9" s="14">
-        <f>SUM(J9:J8)</f>
-      </c>
-      <c r="K9" s="14">
-        <f>SUM(K9:K8)</f>
-      </c>
-      <c r="L9" s="14">
-        <f>SUM(L9:L8)</f>
-      </c>
+      <c r="B9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="16">
+        <v>20</v>
+      </c>
+      <c r="F9" s="16">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="14">
-        <f>SUM(E7:E8)</f>
-      </c>
-      <c r="F10" s="14">
-        <f>SUM(F7:F8)</f>
-      </c>
-      <c r="G10" s="14">
-        <f>SUM(G7:G8)</f>
-      </c>
-      <c r="H10" s="14">
-        <f>SUM(H7:H8)</f>
-      </c>
-      <c r="I10" s="14">
-        <f>SUM(I7:I8)</f>
-      </c>
-      <c r="J10" s="14">
-        <f>SUM(J7:J8)</f>
-      </c>
-      <c r="K10" s="14">
-        <f>SUM(K7:K8)</f>
-      </c>
-      <c r="L10" s="14">
-        <f>SUM(L7:L8)</f>
+      <c r="A10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="16">
+        <v>15</v>
+      </c>
+      <c r="K10" s="16">
+        <v>12</v>
+      </c>
+      <c r="L10" s="16">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="A11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="14">
+        <f>SUM(E9:E10)</f>
+      </c>
+      <c r="F11" s="14">
+        <f>SUM(F9:F10)</f>
+      </c>
+      <c r="G11" s="14">
+        <f>SUM(G9:G10)</f>
+      </c>
+      <c r="H11" s="14">
+        <f>SUM(H9:H10)</f>
+      </c>
+      <c r="I11" s="14">
+        <f>SUM(I9:I10)</f>
+      </c>
+      <c r="J11" s="14">
+        <f>SUM(J9:J10)</f>
+      </c>
+      <c r="K11" s="14">
+        <f>SUM(K9:K10)</f>
+      </c>
+      <c r="L11" s="14">
+        <f>SUM(L9:L10)</f>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E12" s="14">
-        <f>SUM(E12:E11)</f>
+        <f>SUM(E7:E10)</f>
       </c>
       <c r="F12" s="14">
-        <f>SUM(F12:F11)</f>
+        <f>SUM(F7:F10)</f>
       </c>
       <c r="G12" s="14">
-        <f>SUM(G12:G11)</f>
+        <f>SUM(G7:G10)</f>
       </c>
       <c r="H12" s="14">
-        <f>SUM(H12:H11)</f>
+        <f>SUM(H7:H10)</f>
       </c>
       <c r="I12" s="14">
-        <f>SUM(I12:I11)</f>
+        <f>SUM(I7:I10)</f>
       </c>
       <c r="J12" s="14">
-        <f>SUM(J12:J11)</f>
+        <f>SUM(J7:J10)</f>
       </c>
       <c r="K12" s="14">
-        <f>SUM(K12:K11)</f>
+        <f>SUM(K7:K10)</f>
       </c>
       <c r="L12" s="14">
-        <f>SUM(L12:L11)</f>
+        <f>SUM(L7:L10)</f>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="14">
-        <f>E10-E12</f>
-      </c>
-      <c r="F13" s="14">
-        <f>F10-F12</f>
-      </c>
-      <c r="G13" s="14">
-        <f>G10-G12</f>
-      </c>
-      <c r="H13" s="14">
-        <f>H10-H12</f>
-      </c>
-      <c r="I13" s="14">
-        <f>I10-I12</f>
-      </c>
-      <c r="J13" s="14">
-        <f>J10-J12</f>
-      </c>
-      <c r="K13" s="14">
-        <f>K10-K12</f>
-      </c>
-      <c r="L13" s="14">
-        <f>L10-L12</f>
+      <c r="A13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="16">
+        <v>3</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="14">
+        <f>SUM(E14:E14)</f>
+      </c>
+      <c r="F15" s="14">
+        <f>SUM(F14:F14)</f>
+      </c>
+      <c r="G15" s="14">
+        <f>SUM(G14:G14)</f>
+      </c>
+      <c r="H15" s="14">
+        <f>SUM(H14:H14)</f>
+      </c>
+      <c r="I15" s="14">
+        <f>SUM(I14:I14)</f>
+      </c>
+      <c r="J15" s="14">
+        <f>SUM(J14:J14)</f>
+      </c>
+      <c r="K15" s="14">
+        <f>SUM(K14:K14)</f>
+      </c>
+      <c r="L15" s="14">
+        <f>SUM(L14:L14)</f>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="14">
+        <f>E12-E15</f>
+      </c>
+      <c r="F16" s="14">
+        <f>F12-F15</f>
+      </c>
+      <c r="G16" s="14">
+        <f>G12-G15</f>
+      </c>
+      <c r="H16" s="14">
+        <f>H12-H15</f>
+      </c>
+      <c r="I16" s="14">
+        <f>I12-I15</f>
+      </c>
+      <c r="J16" s="14">
+        <f>J12-J15</f>
+      </c>
+      <c r="K16" s="14">
+        <f>K12-K15</f>
+      </c>
+      <c r="L16" s="14">
+        <f>L12-L15</f>
       </c>
     </row>
   </sheetData>
@@ -802,25 +926,28 @@
     <mergeCell ref="L6"/>
     <mergeCell ref="L7"/>
     <mergeCell ref="E1:L1"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A9"/>
+    <mergeCell ref="B9"/>
+    <mergeCell ref="C9"/>
+    <mergeCell ref="D9"/>
     <mergeCell ref="E9"/>
     <mergeCell ref="F9"/>
-    <mergeCell ref="G9"/>
-    <mergeCell ref="H9"/>
-    <mergeCell ref="I9"/>
-    <mergeCell ref="J9"/>
-    <mergeCell ref="K9"/>
-    <mergeCell ref="L9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10"/>
-    <mergeCell ref="F10"/>
-    <mergeCell ref="G10"/>
-    <mergeCell ref="H10"/>
-    <mergeCell ref="I10"/>
+    <mergeCell ref="A10"/>
+    <mergeCell ref="B10"/>
+    <mergeCell ref="C10"/>
+    <mergeCell ref="D10"/>
     <mergeCell ref="J10"/>
     <mergeCell ref="K10"/>
     <mergeCell ref="L10"/>
     <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11"/>
+    <mergeCell ref="F11"/>
+    <mergeCell ref="G11"/>
+    <mergeCell ref="H11"/>
+    <mergeCell ref="I11"/>
+    <mergeCell ref="J11"/>
+    <mergeCell ref="K11"/>
+    <mergeCell ref="L11"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="E12"/>
     <mergeCell ref="F12"/>
@@ -831,14 +958,29 @@
     <mergeCell ref="K12"/>
     <mergeCell ref="L12"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13"/>
-    <mergeCell ref="F13"/>
-    <mergeCell ref="G13"/>
-    <mergeCell ref="H13"/>
-    <mergeCell ref="I13"/>
-    <mergeCell ref="J13"/>
-    <mergeCell ref="K13"/>
-    <mergeCell ref="L13"/>
+    <mergeCell ref="A14"/>
+    <mergeCell ref="B14"/>
+    <mergeCell ref="C14"/>
+    <mergeCell ref="D14"/>
+    <mergeCell ref="E14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="E15"/>
+    <mergeCell ref="F15"/>
+    <mergeCell ref="G15"/>
+    <mergeCell ref="H15"/>
+    <mergeCell ref="I15"/>
+    <mergeCell ref="J15"/>
+    <mergeCell ref="K15"/>
+    <mergeCell ref="L15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16"/>
+    <mergeCell ref="F16"/>
+    <mergeCell ref="G16"/>
+    <mergeCell ref="H16"/>
+    <mergeCell ref="I16"/>
+    <mergeCell ref="J16"/>
+    <mergeCell ref="K16"/>
+    <mergeCell ref="L16"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>